<commit_message>
- new papers: Dunin-Barkowskii, one of the Hopfield papers about short-term memory
</commit_message>
<xml_diff>
--- a/trunk/Список прочитанных статей.xlsx
+++ b/trunk/Список прочитанных статей.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="10332" windowHeight="8388"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="10335" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2051" uniqueCount="1934">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2060" uniqueCount="1943">
   <si>
     <t>НАЗВАНИЕ</t>
   </si>
@@ -5819,6 +5819,33 @@
   </si>
   <si>
     <t>Если применять STDP с отрицательным интегралом + простое повышение веса от частоты, то для частотных нейронов выравниевается эффективность синапсов - те синапсы, которые стоят раньше имеют больший вес, тем те что стоят около постспайка - их влияние на спайк выравнивается</t>
+  </si>
+  <si>
+    <t>Hebb-Hopfield neural networks based on one-dimensional sets of neuron states</t>
+  </si>
+  <si>
+    <t>Witali L. Dunin-Barkowski, Natali B. Osovets</t>
+  </si>
+  <si>
+    <t>Сеть из простых пороговых нейронов, соединенных близко к Хопфилдским (автоасооциативным) имеет аттрактор в динамике - нейроны стабилизируются на частотах. Если добавить понижение чуствительности после активности, то нейроны передают активность по цепочке - возникают медленные цепи-циклы активности</t>
+  </si>
+  <si>
+    <t>NEURAL NETWORK WITH FORMED DYNAMICS OF ACTIVITY</t>
+  </si>
+  <si>
+    <t>V. L. Dunin-Barkovskii and N. B. Osovets</t>
+  </si>
+  <si>
+    <t>Хаотические сети из упрощенных дискретных временных пороговых нейронов могут показывать стационарную активность с динамическими аттракторами (а не хаос)</t>
+  </si>
+  <si>
+    <t>Sequence reproduction, single trial learning, and mimicry based on a mammalian-like distributed code for time</t>
+  </si>
+  <si>
+    <t>J. J. Hopfield1 and Carlos D. Brody</t>
+  </si>
+  <si>
+    <t>Есть нейроны с медленно меняющейся активностью - порядка несколько секунд. С помощью этих нейронов другие нейроны с помощью гамма-ритма активируются в строго определенные моменты времени. С помощью этих двух слоев можно всегда спросить у сети сколько времени? Третий слой один раз учится отображать время и стимул на активаторы - получаем кратковременную память: один раз показали, сеть повторяет мелодию.</t>
   </si>
 </sst>
 </file>
@@ -5862,7 +5889,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -5875,6 +5902,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -6171,18 +6201,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C60"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="44.1" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="44.1" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="47.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="64.44140625" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="47.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="64.42578125" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="44.1" customHeight="1">
@@ -6845,9 +6875,42 @@
         <v>1933</v>
       </c>
     </row>
+    <row r="61" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A61" s="1" t="s">
+        <v>1934</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>1935</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>1936</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A62" s="6" t="s">
+        <v>1937</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>1938</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>1939</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A63" s="1" t="s">
+        <v>1940</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>1941</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>1942</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6859,12 +6922,12 @@
       <selection activeCell="A457" sqref="A457"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="44.1" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="44.1" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="47.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="64.44140625" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="47.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="64.42578125" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="44.1" customHeight="1">
@@ -13545,12 +13608,12 @@
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="96" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="96" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="33.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="27.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="69.33203125" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.109375" style="3"/>
+    <col min="1" max="1" width="33.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="69.28515625" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="96" customHeight="1">

</xml_diff>

<commit_message>
- Code-specific policy gradient rules for spiking neurons.pdf
</commit_message>
<xml_diff>
--- a/trunk/Список прочитанных статей.xlsx
+++ b/trunk/Список прочитанных статей.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2087" uniqueCount="1970">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2089" uniqueCount="1972">
   <si>
     <t>НАЗВАНИЕ</t>
   </si>
@@ -5927,6 +5927,12 @@
   </si>
   <si>
     <t>ReSuMe</t>
+  </si>
+  <si>
+    <t>Code-specific policy gradient rules for spiking neurons</t>
+  </si>
+  <si>
+    <t>H. Sprekeler, G. Hennequin, W. Gerstner</t>
   </si>
 </sst>
 </file>
@@ -6282,18 +6288,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C72"/>
+  <dimension ref="A1:C73"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72:C72"/>
+      <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="44.1" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="47.109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="24.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="64.44140625" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.109375" style="1"/>
+    <col min="3" max="3" width="45.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="44.1" customHeight="1">
@@ -7086,6 +7093,14 @@
       </c>
       <c r="C72" s="1" t="s">
         <v>1969</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A73" s="1" t="s">
+        <v>1970</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>1971</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- reinforcement/Reinforcement learning Computational theory and biological mechanisms.pdf
</commit_message>
<xml_diff>
--- a/trunk/Список прочитанных статей.xlsx
+++ b/trunk/Список прочитанных статей.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2089" uniqueCount="1972">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2093" uniqueCount="1976">
   <si>
     <t>НАЗВАНИЕ</t>
   </si>
@@ -5932,7 +5932,19 @@
     <t>Code-specific policy gradient rules for spiking neurons</t>
   </si>
   <si>
-    <t>H. Sprekeler, G. Hennequin, W. Gerstner</t>
+    <t>Градиентным спуском увеличивать ожидаемое значение награды, но для разных coding features: отдельное правило для общей частоты, отдельное для паттерна</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H. Sprekeler, G. Hennequin, W. Gerstner; Advances in Neural Information Processing Systems 22 (NIPS 2009) </t>
+  </si>
+  <si>
+    <t>Reinforcement learning: Computational theory and biological mechanisms</t>
+  </si>
+  <si>
+    <t>K. Doya; 2007, HFSP Journal, 1, 30-40</t>
+  </si>
+  <si>
+    <t>Обзор обучения с подкреплением и его реализации в мозге. У них есть вроде полная теория где что находится</t>
   </si>
 </sst>
 </file>
@@ -6288,10 +6300,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C73"/>
+  <dimension ref="A1:C74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="44.1" customHeight="1"/>
@@ -7100,7 +7112,21 @@
         <v>1970</v>
       </c>
       <c r="B73" s="1" t="s">
+        <v>1972</v>
+      </c>
+      <c r="C73" s="1" t="s">
         <v>1971</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A74" s="1" t="s">
+        <v>1973</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>1974</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>1975</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- reinforcement/Reinforcement Learning With Modulated Spike Timing–Dependent Synaptic Plasticity.pdf
</commit_message>
<xml_diff>
--- a/trunk/Список прочитанных статей.xlsx
+++ b/trunk/Список прочитанных статей.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2093" uniqueCount="1976">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2096" uniqueCount="1979">
   <si>
     <t>НАЗВАНИЕ</t>
   </si>
@@ -5945,6 +5945,15 @@
   </si>
   <si>
     <t>Обзор обучения с подкреплением и его реализации в мозге. У них есть вроде полная теория где что находится</t>
+  </si>
+  <si>
+    <t>Reinforcement Learning With Modulated Spike Timing–Dependent Synaptic Plasticity</t>
+  </si>
+  <si>
+    <t>M. A. Farries, A. L. Fairhall; J Neurophysiol 98: 3648-3665, 2007</t>
+  </si>
+  <si>
+    <t>"Подкрпление" вычисляется как расхождение нужного спайка и спайка нейрона и посылается гипотетической системой в момент когда спайк нужен - чистое обучение с учителем. Изобилие технических деталей их экспериментов</t>
   </si>
 </sst>
 </file>
@@ -6300,10 +6309,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C74"/>
+  <dimension ref="A1:C75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="44.1" customHeight="1"/>
@@ -7127,6 +7136,17 @@
       </c>
       <c r="C74" s="1" t="s">
         <v>1975</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A75" s="1" t="s">
+        <v>1976</v>
+      </c>
+      <c r="B75" t="s">
+        <v>1977</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>1978</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- a learning theory of MSTDP
</commit_message>
<xml_diff>
--- a/trunk/Список прочитанных статей.xlsx
+++ b/trunk/Список прочитанных статей.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2096" uniqueCount="1979">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2099" uniqueCount="1982">
   <si>
     <t>НАЗВАНИЕ</t>
   </si>
@@ -5954,6 +5954,15 @@
   </si>
   <si>
     <t>"Подкрпление" вычисляется как расхождение нужного спайка и спайка нейрона и посылается гипотетической системой в момент когда спайк нужен - чистое обучение с учителем. Изобилие технических деталей их экспериментов</t>
+  </si>
+  <si>
+    <t>A Learning Theory for Reward-Modulated Spike-Timing-Dependent Plasticity with Application to Biofeedback</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R. Legenstein, D. Pecevski, W. Maass; PLoS Comput Biol. 2008 Oct;4(10) </t>
+  </si>
+  <si>
+    <t>Большая работа по применению MSTDP в тестовых задачах за награду: увеличить частоту, повторить паттерн, различить два входных паттерна, различиьт речь. Много осредненной математики по MSTDP</t>
   </si>
 </sst>
 </file>
@@ -6309,10 +6318,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C75"/>
+  <dimension ref="A1:C76"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="44.1" customHeight="1"/>
@@ -7147,6 +7156,17 @@
       </c>
       <c r="C75" s="1" t="s">
         <v>1978</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A76" s="1" t="s">
+        <v>1979</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>1980</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>1981</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Functional Requirements for Reward-Modulated Spike-Timing-Dependent Plasticity.pdf
</commit_message>
<xml_diff>
--- a/trunk/Список прочитанных статей.xlsx
+++ b/trunk/Список прочитанных статей.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2099" uniqueCount="1982">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2102" uniqueCount="1985">
   <si>
     <t>НАЗВАНИЕ</t>
   </si>
@@ -5963,6 +5963,15 @@
   </si>
   <si>
     <t>Большая работа по применению MSTDP в тестовых задачах за награду: увеличить частоту, повторить паттерн, различить два входных паттерна, различиьт речь. Много осредненной математики по MSTDP</t>
+  </si>
+  <si>
+    <t>Functional Requirements for Reward-Modulated Spike-Timing-Dependent Plasticity</t>
+  </si>
+  <si>
+    <t>N. Fremaux, H. Sprekeler, and W. Gerstner; The Journal of Neuroscience, October 6, 2010, 30(40)</t>
+  </si>
+  <si>
+    <t>Очень хорошая статья про нюансы RSTDP. Правило с модуляцией можно разложить на часть с самообучением и часть с наградой. У простого STDP есть часть с самообучением - поэтому возникает шифт при изменении базового уровня награды. Этот сдвиг исчезает при применении критика: d = Rexp - R. Правило R-max (теоретическое) лищено шифта.</t>
   </si>
 </sst>
 </file>
@@ -6318,10 +6327,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C76"/>
+  <dimension ref="A1:C77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="C77" sqref="C77"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="C78" sqref="C78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="44.1" customHeight="1"/>
@@ -7167,6 +7176,17 @@
       </c>
       <c r="C76" s="1" t="s">
         <v>1981</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A77" s="1" t="s">
+        <v>1982</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>1983</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>1984</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- reinforcement/Reinforcement Learning, Spike Time Dependent Plasticity and the BCM Rule.pdf
</commit_message>
<xml_diff>
--- a/trunk/Список прочитанных статей.xlsx
+++ b/trunk/Список прочитанных статей.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2102" uniqueCount="1985">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2105" uniqueCount="1988">
   <si>
     <t>НАЗВАНИЕ</t>
   </si>
@@ -5972,6 +5972,15 @@
   </si>
   <si>
     <t>Очень хорошая статья про нюансы RSTDP. Правило с модуляцией можно разложить на часть с самообучением и часть с наградой. У простого STDP есть часть с самообучением - поэтому возникает шифт при изменении базового уровня награды. Этот сдвиг исчезает при применении критика: d = Rexp - R. Правило R-max (теоретическое) лищено шифта.</t>
+  </si>
+  <si>
+    <t>Reinforcement Learning, Spike Time Dependent Plasticity and the BCM Rule</t>
+  </si>
+  <si>
+    <t>D. Baras , R. Meir ; Neural Comput. 2007 Aug;19(8)</t>
+  </si>
+  <si>
+    <t>На основе Baxter по другому формулируют reinforcement learning for stochastic IF. Состояния - напряжение, политика - паттерн в дискретном времени. Я думаю, что они неправильно представили вероятность паттерна, поэтому они на прямую дифф. сигмоид. Полученные правила тестируют на xor и на нахождении пути в маленькой сети от входного нейрона до выходного.</t>
   </si>
 </sst>
 </file>
@@ -6327,10 +6336,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C77"/>
+  <dimension ref="A1:C78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="C78" sqref="C78"/>
+      <selection activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="44.1" customHeight="1"/>
@@ -7187,6 +7196,17 @@
       </c>
       <c r="C77" s="1" t="s">
         <v>1984</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A78" s="1" t="s">
+        <v>1985</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>1986</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>1987</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Training networks of biological realistic spiking neurons for real-time robot control.pdf
</commit_message>
<xml_diff>
--- a/trunk/Список прочитанных статей.xlsx
+++ b/trunk/Список прочитанных статей.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2105" uniqueCount="1988">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2108" uniqueCount="1991">
   <si>
     <t>НАЗВАНИЕ</t>
   </si>
@@ -5981,6 +5981,15 @@
   </si>
   <si>
     <t>На основе Baxter по другому формулируют reinforcement learning for stochastic IF. Состояния - напряжение, политика - паттерн в дискретном времени. Я думаю, что они неправильно представили вероятность паттерна, поэтому они на прямую дифф. сигмоид. Полученные правила тестируют на xor и на нахождении пути в маленькой сети от входного нейрона до выходного.</t>
+  </si>
+  <si>
+    <t>Training networks of biological realistic spiking neurons for real-time robot control</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H. Burgsteiner, (2005). Proceedings of the 9th International Conference on Engineering Applications of Neural Networks, Lile, France  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">LSM для объезда препядствий khepera. </t>
   </si>
 </sst>
 </file>
@@ -6336,10 +6345,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C78"/>
+  <dimension ref="A1:C79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78"/>
+      <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="44.1" customHeight="1"/>
@@ -7207,6 +7216,17 @@
       </c>
       <c r="C78" s="1" t="s">
         <v>1987</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A79" s="1" t="s">
+        <v>1988</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>1989</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>1990</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Evolving Spiking Neurons from Wheels to Wings.pdf
</commit_message>
<xml_diff>
--- a/trunk/Список прочитанных статей.xlsx
+++ b/trunk/Список прочитанных статей.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2108" uniqueCount="1991">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2111" uniqueCount="1994">
   <si>
     <t>НАЗВАНИЕ</t>
   </si>
@@ -5990,6 +5990,15 @@
   </si>
   <si>
     <t xml:space="preserve">LSM для объезда препядствий khepera. </t>
+  </si>
+  <si>
+    <t>Evolving Spiking Neurons from Wheels to Wings</t>
+  </si>
+  <si>
+    <t>D. Floreano, J.-C. Zufferey, C. Mattiussi;Dynamic Systems Approach for Embodiment and Sociality, vol. 6, 2003, p. 65-70</t>
+  </si>
+  <si>
+    <t>Маленикий обзор их работ по evolving SNN</t>
   </si>
 </sst>
 </file>
@@ -6345,10 +6354,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C79"/>
+  <dimension ref="A1:C80"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79"/>
+      <selection activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="44.1" customHeight="1"/>
@@ -7227,6 +7236,17 @@
       </c>
       <c r="C79" s="1" t="s">
         <v>1990</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A80" s="1" t="s">
+        <v>1991</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>1992</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>1993</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Mobile Robot Control in the Road Sign Problem using Reservoir Computing Networks.pdf
</commit_message>
<xml_diff>
--- a/trunk/Список прочитанных статей.xlsx
+++ b/trunk/Список прочитанных статей.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2111" uniqueCount="1994">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2114" uniqueCount="1997">
   <si>
     <t>НАЗВАНИЕ</t>
   </si>
@@ -5999,6 +5999,15 @@
   </si>
   <si>
     <t>Маленикий обзор их работ по evolving SNN</t>
+  </si>
+  <si>
+    <t>Mobile Robot Control in the Road Sign Problem using Reservoir Computing Networks</t>
+  </si>
+  <si>
+    <t>E. A. Antonelo, B. Schrauwen, D. Stroobandt; IEEE Int. Conf. on Robotics and Automation (ICRA), 2008</t>
+  </si>
+  <si>
+    <t>LSM для Tmaze с цветными знаками</t>
   </si>
 </sst>
 </file>
@@ -6354,10 +6363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C80"/>
+  <dimension ref="A1:C81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="A80" sqref="A80"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="44.1" customHeight="1"/>
@@ -7247,6 +7256,17 @@
       </c>
       <c r="C80" s="1" t="s">
         <v>1993</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A81" s="1" t="s">
+        <v>1994</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>1995</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>1996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Spike-time robotics a rapid response circuit for a robot that seeks temporally varying stimuli.pdf
</commit_message>
<xml_diff>
--- a/trunk/Список прочитанных статей.xlsx
+++ b/trunk/Список прочитанных статей.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2114" uniqueCount="1997">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2117" uniqueCount="2000">
   <si>
     <t>НАЗВАНИЕ</t>
   </si>
@@ -6008,6 +6008,15 @@
   </si>
   <si>
     <t>LSM для Tmaze с цветными знаками</t>
+  </si>
+  <si>
+    <t>Spike-time robotics: a rapid response circuit for a robot that seeks temporally varying stimuli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J. Wiles, D. Ball, S. Heath, C. Nolan, P. Stratton; Australian Journal of Intelligent Information Processing Systems, 2010. </t>
+  </si>
+  <si>
+    <t>Цепочка из кортекса: inh n + exc + немного настраиваемые параметры для фототаксиса вроде</t>
   </si>
 </sst>
 </file>
@@ -6363,10 +6372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C81"/>
+  <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="44.1" customHeight="1"/>
@@ -7267,6 +7276,17 @@
       </c>
       <c r="C81" s="1" t="s">
         <v>1996</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A82" s="1" t="s">
+        <v>1997</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>1998</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>1999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Movement Generation with Circuits of Spiking Neurons.pdf
</commit_message>
<xml_diff>
--- a/trunk/Список прочитанных статей.xlsx
+++ b/trunk/Список прочитанных статей.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2117" uniqueCount="2000">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2120" uniqueCount="2003">
   <si>
     <t>НАЗВАНИЕ</t>
   </si>
@@ -6017,6 +6017,15 @@
   </si>
   <si>
     <t>Цепочка из кортекса: inh n + exc + немного настраиваемые параметры для фототаксиса вроде</t>
+  </si>
+  <si>
+    <t>Movement Generation with Circuits of Spiking Neurons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P. Joshi, W. Maass; Neural Computation, 17(8):1715-1738, 2005. </t>
+  </si>
+  <si>
+    <t>LSM. Манипулятор обучают траекториям. Сначала берут траекторию и генерируют обратные связи, как будто сеть уже правильно выполняет (на основе модели). Потом обр. связи идут реальные</t>
   </si>
 </sst>
 </file>
@@ -6372,10 +6381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C82"/>
+  <dimension ref="A1:C83"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82"/>
+      <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="44.1" customHeight="1"/>
@@ -7287,6 +7296,17 @@
       </c>
       <c r="C82" s="1" t="s">
         <v>1999</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A83" s="1" t="s">
+        <v>2000</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>2001</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>2002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- reinforcement/Reinforcement Learning with Long Short-Term Memory.pdf
</commit_message>
<xml_diff>
--- a/trunk/Список прочитанных статей.xlsx
+++ b/trunk/Список прочитанных статей.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2120" uniqueCount="2003">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2123" uniqueCount="2006">
   <si>
     <t>НАЗВАНИЕ</t>
   </si>
@@ -6026,6 +6026,15 @@
   </si>
   <si>
     <t>LSM. Манипулятор обучают траекториям. Сначала берут траекторию и генерируют обратные связи, как будто сеть уже правильно выполняет (на основе модели). Потом обр. связи идут реальные</t>
+  </si>
+  <si>
+    <t>B. Bakker; Advances in Neural Information Processing Systems 13 (NIPS'13), 2002</t>
+  </si>
+  <si>
+    <t>Reinforcement Learning with Long Short-Term Memory</t>
+  </si>
+  <si>
+    <t>Архитектура для онлайн обучения с подкреплением для сигмоидальных частотных сетей</t>
   </si>
 </sst>
 </file>
@@ -6381,10 +6390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C83"/>
+  <dimension ref="A1:C84"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+      <selection activeCell="A84" sqref="A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="44.1" customHeight="1"/>
@@ -7307,6 +7316,17 @@
       </c>
       <c r="C83" s="1" t="s">
         <v>2002</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A84" t="s">
+        <v>2004</v>
+      </c>
+      <c r="B84" t="s">
+        <v>2003</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>2005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ARBIB an Autonomous Robot Based on Inspirations from Biology.pdf + similar work
</commit_message>
<xml_diff>
--- a/trunk/Список прочитанных статей.xlsx
+++ b/trunk/Список прочитанных статей.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2123" uniqueCount="2006">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2129" uniqueCount="2012">
   <si>
     <t>НАЗВАНИЕ</t>
   </si>
@@ -6035,6 +6035,24 @@
   </si>
   <si>
     <t>Архитектура для онлайн обучения с подкреплением для сигмоидальных частотных сетей</t>
+  </si>
+  <si>
+    <t>ARBIB: an Autonomous Robot Based on Inspirations from Biology</t>
+  </si>
+  <si>
+    <t>R. I. Damper ,  R. L. B. French ,  T. W. Scutt; Robotics and Autonomous Systems, 31 (4). pp. 247-274</t>
+  </si>
+  <si>
+    <t>Applisia-like для объезда препятсвий с датчиками света (не дочитал)</t>
+  </si>
+  <si>
+    <t>A Simple Aplysia-Like Spiking Neural Network to Generate Adaptive Behavior in Autonomous Robots</t>
+  </si>
+  <si>
+    <t>F. Alnajjar; K. Murase; Adaptive Behavior June 1, 2009 17: 179-196</t>
+  </si>
+  <si>
+    <t>Полной версии в свободном доступе нет. Трехслойная SRM сеть. Внутренний слой модулируется от сенсоров. Прошитые рефлексы изменяются - объезд препятсвий со светом</t>
   </si>
 </sst>
 </file>
@@ -6390,10 +6408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C84"/>
+  <dimension ref="A1:C86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="A84" sqref="A84"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="C87" sqref="C87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="44.1" customHeight="1"/>
@@ -7327,6 +7345,28 @@
       </c>
       <c r="C84" s="1" t="s">
         <v>2005</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A85" s="1" t="s">
+        <v>2006</v>
+      </c>
+      <c r="B85" t="s">
+        <v>2007</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A86" s="1" t="s">
+        <v>2009</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>2010</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>2011</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- reinforcement/Reinforcement Learning of a Simple Control Task Using the Spike Response Model.pdf
</commit_message>
<xml_diff>
--- a/trunk/Список прочитанных статей.xlsx
+++ b/trunk/Список прочитанных статей.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2129" uniqueCount="2012">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2134" uniqueCount="2017">
   <si>
     <t>НАЗВАНИЕ</t>
   </si>
@@ -6053,6 +6053,21 @@
   </si>
   <si>
     <t>Полной версии в свободном доступе нет. Трехслойная SRM сеть. Внутренний слой модулируется от сенсоров. Прошитые рефлексы изменяются - объезд препятсвий со светом</t>
+  </si>
+  <si>
+    <t>Spikes: Exploring the Neural Code (Computational Neuroscience)</t>
+  </si>
+  <si>
+    <t>Не читал, но выглядит хорошо</t>
+  </si>
+  <si>
+    <t>F. Rieke, D. Warland, R. Ruyter van Steveninck, W. Bialek; Computational Neurosciences series. MIT Press, 1997</t>
+  </si>
+  <si>
+    <t>Reinforcement Learning of a Simple Control Task Using the Spike Response Model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M. S. Queiroz, A. Braga, R. C. Berredo, Neurocomputing, Vol. 70, Issues 1-3, Pages 14-20 </t>
   </si>
 </sst>
 </file>
@@ -6408,10 +6423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C86"/>
+  <dimension ref="A1:C88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="C87" sqref="C87"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="B88" sqref="B88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="44.1" customHeight="1"/>
@@ -7367,6 +7382,25 @@
       </c>
       <c r="C86" s="1" t="s">
         <v>2011</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A87" s="1" t="s">
+        <v>2012</v>
+      </c>
+      <c r="B87" t="s">
+        <v>2014</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A88" s="1" t="s">
+        <v>2015</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>2016</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Efficient temporal processing with biologically realistic dynamic synapses.pdf
</commit_message>
<xml_diff>
--- a/trunk/Список прочитанных статей.xlsx
+++ b/trunk/Список прочитанных статей.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2134" uniqueCount="2017">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2138" uniqueCount="2021">
   <si>
     <t>НАЗВАНИЕ</t>
   </si>
@@ -6068,6 +6068,18 @@
   </si>
   <si>
     <t xml:space="preserve">M. S. Queiroz, A. Braga, R. C. Berredo, Neurocomputing, Vol. 70, Issues 1-3, Pages 14-20 </t>
+  </si>
+  <si>
+    <t>Baxter подход к обучению с подкреплением. Как я думаю не правильный вывод (получили не энтропию). Многосинапсный нейрон с задержками. Применение: обучение тележки в горку как к Barto. Кодируется скорость и позиция с помощью времени спайков. Награда всегда -1, а в конце +1.</t>
+  </si>
+  <si>
+    <t>Efficient temporal processing with biologically realistic dynamic synapses</t>
+  </si>
+  <si>
+    <t>T. Natschlaeger, W. Maass, and A. Zador; Network: Computation in Neural Systems, 12:75-87, 2001</t>
+  </si>
+  <si>
+    <t>Разные синапсы как разные дин. Фильтры для частотного нейрона. Есть универсальная апроксимационная теорема для функции, разложенной по фильтрам</t>
   </si>
 </sst>
 </file>
@@ -6423,10 +6435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C88"/>
+  <dimension ref="A1:C89"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="B88" sqref="B88"/>
+      <selection activeCell="A89" sqref="A89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="44.1" customHeight="1"/>
@@ -7401,6 +7413,20 @@
       </c>
       <c r="B88" s="1" t="s">
         <v>2016</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A89" s="1" t="s">
+        <v>2018</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>2019</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>2020</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Synaptic plasticity model of a spiking neural network for reinforcement learning.pdf
</commit_message>
<xml_diff>
--- a/trunk/Список прочитанных статей.xlsx
+++ b/trunk/Список прочитанных статей.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2138" uniqueCount="2021">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2141" uniqueCount="2024">
   <si>
     <t>НАЗВАНИЕ</t>
   </si>
@@ -5848,9 +5848,6 @@
     <t>Reinforcement learning through modulation of spike-timing-dependent synaptic plasticity</t>
   </si>
   <si>
-    <t>Razvan V. Florian</t>
-  </si>
-  <si>
     <t>MSTDP выведено на основе OLPOMDP (Baxter). Все сходится с тем, что исползую: функция забывания, минимизация энтропии. Эксперименты в статье не очень - XOR, частотные</t>
   </si>
   <si>
@@ -6080,6 +6077,18 @@
   </si>
   <si>
     <t>Разные синапсы как разные дин. Фильтры для частотного нейрона. Есть универсальная апроксимационная теорема для функции, разложенной по фильтрам</t>
+  </si>
+  <si>
+    <t>Razvan V. Florian; Neural Comput. 2007 Jun;19(6):1468-502.</t>
+  </si>
+  <si>
+    <t>Synaptic plasticity model of a spiking neural network for reinforcement learning</t>
+  </si>
+  <si>
+    <t>Kyoobin Lee, Dong-Soo Kwon; Neurocomputing Vol. 71, Issues 13-15, August 2008, Pages 3037-3043</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Эвристическое (но правильное) обучение с подкреплением для SRM сети на примере агента в дискретной сетке 9х9 (как у меня) </t>
   </si>
 </sst>
 </file>
@@ -6435,10 +6444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C89"/>
+  <dimension ref="A1:C90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="A89" sqref="A89"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="44.1" customHeight="1"/>
@@ -7093,7 +7102,7 @@
         <v>1928</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>1966</v>
+        <v>1965</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>1929</v>
@@ -7148,285 +7157,296 @@
         <v>1942</v>
       </c>
       <c r="B64" s="1" t="s">
+        <v>2020</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>1943</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>1944</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="44.1" customHeight="1">
       <c r="A65" s="1" t="s">
+        <v>1944</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>1945</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="C65" s="1" t="s">
         <v>1946</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>1947</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="44.1" customHeight="1">
       <c r="A66" s="1" t="s">
+        <v>1947</v>
+      </c>
+      <c r="B66" s="1" t="s">
         <v>1948</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="C66" s="1" t="s">
         <v>1949</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>1950</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="44.1" customHeight="1">
       <c r="A67" s="1" t="s">
+        <v>1950</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>1951</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="C67" s="1" t="s">
         <v>1952</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>1953</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="44.1" customHeight="1">
       <c r="A68" s="1" t="s">
-        <v>1956</v>
+        <v>1955</v>
       </c>
       <c r="B68" s="1" t="s">
+        <v>1953</v>
+      </c>
+      <c r="C68" s="1" t="s">
         <v>1954</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>1955</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="44.1" customHeight="1">
       <c r="A69" s="1" t="s">
+        <v>1956</v>
+      </c>
+      <c r="B69" s="1" t="s">
         <v>1957</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="C69" s="1" t="s">
         <v>1958</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>1959</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="44.1" customHeight="1">
       <c r="A70" s="1" t="s">
+        <v>1959</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>1960</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="C70" s="1" t="s">
         <v>1961</v>
-      </c>
-      <c r="C70" s="1" t="s">
-        <v>1962</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="44.1" customHeight="1">
       <c r="A71" s="1" t="s">
+        <v>1962</v>
+      </c>
+      <c r="B71" s="1" t="s">
         <v>1963</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="C71" s="1" t="s">
         <v>1964</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>1965</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="44.1" customHeight="1">
       <c r="A72" s="1" t="s">
+        <v>1966</v>
+      </c>
+      <c r="B72" s="1" t="s">
         <v>1967</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="C72" s="1" t="s">
         <v>1968</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>1969</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="44.1" customHeight="1">
       <c r="A73" s="1" t="s">
+        <v>1969</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>1971</v>
+      </c>
+      <c r="C73" s="1" t="s">
         <v>1970</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>1972</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>1971</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="44.1" customHeight="1">
       <c r="A74" s="1" t="s">
+        <v>1972</v>
+      </c>
+      <c r="B74" s="1" t="s">
         <v>1973</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="C74" s="1" t="s">
         <v>1974</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>1975</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="44.1" customHeight="1">
       <c r="A75" s="1" t="s">
+        <v>1975</v>
+      </c>
+      <c r="B75" t="s">
         <v>1976</v>
       </c>
-      <c r="B75" t="s">
+      <c r="C75" s="1" t="s">
         <v>1977</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>1978</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="44.1" customHeight="1">
       <c r="A76" s="1" t="s">
+        <v>1978</v>
+      </c>
+      <c r="B76" s="1" t="s">
         <v>1979</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="C76" s="1" t="s">
         <v>1980</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>1981</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="44.1" customHeight="1">
       <c r="A77" s="1" t="s">
+        <v>1981</v>
+      </c>
+      <c r="B77" s="1" t="s">
         <v>1982</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="C77" s="1" t="s">
         <v>1983</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>1984</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="44.1" customHeight="1">
       <c r="A78" s="1" t="s">
+        <v>1984</v>
+      </c>
+      <c r="B78" s="1" t="s">
         <v>1985</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="C78" s="1" t="s">
         <v>1986</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>1987</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="44.1" customHeight="1">
       <c r="A79" s="1" t="s">
+        <v>1987</v>
+      </c>
+      <c r="B79" s="1" t="s">
         <v>1988</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="C79" s="1" t="s">
         <v>1989</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>1990</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="44.1" customHeight="1">
       <c r="A80" s="1" t="s">
+        <v>1990</v>
+      </c>
+      <c r="B80" s="1" t="s">
         <v>1991</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="C80" s="1" t="s">
         <v>1992</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>1993</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="44.1" customHeight="1">
       <c r="A81" s="1" t="s">
+        <v>1993</v>
+      </c>
+      <c r="B81" s="1" t="s">
         <v>1994</v>
       </c>
-      <c r="B81" s="1" t="s">
+      <c r="C81" s="1" t="s">
         <v>1995</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>1996</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="44.1" customHeight="1">
       <c r="A82" s="1" t="s">
+        <v>1996</v>
+      </c>
+      <c r="B82" s="1" t="s">
         <v>1997</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="C82" s="1" t="s">
         <v>1998</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>1999</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="44.1" customHeight="1">
       <c r="A83" s="1" t="s">
+        <v>1999</v>
+      </c>
+      <c r="B83" s="1" t="s">
         <v>2000</v>
       </c>
-      <c r="B83" s="1" t="s">
+      <c r="C83" s="1" t="s">
         <v>2001</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>2002</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="44.1" customHeight="1">
       <c r="A84" t="s">
+        <v>2003</v>
+      </c>
+      <c r="B84" t="s">
+        <v>2002</v>
+      </c>
+      <c r="C84" s="1" t="s">
         <v>2004</v>
-      </c>
-      <c r="B84" t="s">
-        <v>2003</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>2005</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="44.1" customHeight="1">
       <c r="A85" s="1" t="s">
+        <v>2005</v>
+      </c>
+      <c r="B85" t="s">
         <v>2006</v>
       </c>
-      <c r="B85" t="s">
+      <c r="C85" s="1" t="s">
         <v>2007</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>2008</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="44.1" customHeight="1">
       <c r="A86" s="1" t="s">
+        <v>2008</v>
+      </c>
+      <c r="B86" s="1" t="s">
         <v>2009</v>
       </c>
-      <c r="B86" s="1" t="s">
+      <c r="C86" s="1" t="s">
         <v>2010</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>2011</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="44.1" customHeight="1">
       <c r="A87" s="1" t="s">
+        <v>2011</v>
+      </c>
+      <c r="B87" t="s">
+        <v>2013</v>
+      </c>
+      <c r="C87" s="1" t="s">
         <v>2012</v>
-      </c>
-      <c r="B87" t="s">
-        <v>2014</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>2013</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="44.1" customHeight="1">
       <c r="A88" s="1" t="s">
+        <v>2014</v>
+      </c>
+      <c r="B88" s="1" t="s">
         <v>2015</v>
       </c>
-      <c r="B88" s="1" t="s">
+      <c r="C88" s="1" t="s">
         <v>2016</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>2017</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="44.1" customHeight="1">
       <c r="A89" s="1" t="s">
+        <v>2017</v>
+      </c>
+      <c r="B89" s="1" t="s">
         <v>2018</v>
       </c>
-      <c r="B89" s="1" t="s">
+      <c r="C89" s="1" t="s">
         <v>2019</v>
       </c>
-      <c r="C89" s="1" t="s">
-        <v>2020</v>
+    </row>
+    <row r="90" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A90" s="1" t="s">
+        <v>2021</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>2022</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>2023</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- reinforcement/A reinforcement learning algorithm for spiking neural networks.pdf
</commit_message>
<xml_diff>
--- a/trunk/Список прочитанных статей.xlsx
+++ b/trunk/Список прочитанных статей.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2141" uniqueCount="2024">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2144" uniqueCount="2027">
   <si>
     <t>НАЗВАНИЕ</t>
   </si>
@@ -6089,6 +6089,15 @@
   </si>
   <si>
     <t xml:space="preserve">Эвристическое (но правильное) обучение с подкреплением для SRM сети на примере агента в дискретной сетке 9х9 (как у меня) </t>
+  </si>
+  <si>
+    <t>A reinforcement learning algorithm for spiking neural networks</t>
+  </si>
+  <si>
+    <t>Razvan V. Florian; SYNASC '05 Proceedings of the Seventh International Symposium on Symbolic and Numeric Algorithms for Scientific Computing, 2005</t>
+  </si>
+  <si>
+    <t>Вывод Florian RSTDP. Применение с нейронами ижикевича, IF и просто MSTDP в задаче: червяк находит еду около норы</t>
   </si>
 </sst>
 </file>
@@ -6444,10 +6453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C90"/>
+  <dimension ref="A1:C91"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="B92" sqref="B92"/>
+      <selection activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="44.1" customHeight="1"/>
@@ -7447,6 +7456,17 @@
       </c>
       <c r="C90" s="1" t="s">
         <v>2023</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A91" s="1" t="s">
+        <v>2024</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>2025</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>2026</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Solving_a_delayed_response_task_with_spiking_and_McCulloch-Pitts_agents.pdf  - Spiking Neural Controllers for Pushing Objects Around.pdf
</commit_message>
<xml_diff>
--- a/trunk/Список прочитанных статей.xlsx
+++ b/trunk/Список прочитанных статей.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2144" uniqueCount="2027">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2150" uniqueCount="2033">
   <si>
     <t>НАЗВАНИЕ</t>
   </si>
@@ -6098,6 +6098,26 @@
   </si>
   <si>
     <t>Вывод Florian RSTDP. Применение с нейронами ижикевича, IF и просто MSTDP в задаче: червяк находит еду около норы</t>
+  </si>
+  <si>
+    <t>Solving a delayed response task with spiking and McCulloch-Pitts agents</t>
+  </si>
+  <si>
+    <t>Saggie, K., Keinan, A., Ruppin, E.; Advances in Artificial Life: 7th European Conference,
+ECAL 2003 Dortmund, Germany, September 14-17, 2003.</t>
+  </si>
+  <si>
+    <t>Как я понял, сравнение бинарных нейроново и IF в задаче обучения с задержкой, где помогает интегрирование на мебмране.</t>
+  </si>
+  <si>
+    <t>Spiking Neural Controllers for Pushing Objects Around</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 
+Razvan V. Florian; In: Lecture Notes in Computer Science, vol. 4095. Springer, Berlin. pp. 570-581</t>
+  </si>
+  <si>
+    <t>Эволюция агента, двигающего шары. STDP чуть помогает, но не сильно, просто делает эволюцию smooth</t>
   </si>
 </sst>
 </file>
@@ -6453,10 +6473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C91"/>
+  <dimension ref="A1:C93"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91"/>
+      <selection activeCell="A93" sqref="A93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="44.1" customHeight="1"/>
@@ -7467,6 +7487,28 @@
       </c>
       <c r="C91" s="1" t="s">
         <v>2026</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A92" s="1" t="s">
+        <v>2027</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>2028</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>2029</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A93" s="1" t="s">
+        <v>2030</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>2031</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>2032</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Learning at the edge of chaos  Temporal Coupling of Spiking Neurons Controller for Autonomous Robotic.pdf
</commit_message>
<xml_diff>
--- a/trunk/Список прочитанных статей.xlsx
+++ b/trunk/Список прочитанных статей.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2150" uniqueCount="2033">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2153" uniqueCount="2036">
   <si>
     <t>НАЗВАНИЕ</t>
   </si>
@@ -6118,6 +6118,15 @@
   </si>
   <si>
     <t>Эволюция агента, двигающего шары. STDP чуть помогает, но не сильно, просто делает эволюцию smooth</t>
+  </si>
+  <si>
+    <t>Learning at the edge of chaos : Temporal Coupling of Spiking Neurons Controller for Autonomous Robotic</t>
+  </si>
+  <si>
+    <t>Soula, H., Alwan, A. and Beslon, G.; Proceedings of American Association for Artificial Intelligence (AAAI) Spring Symposia on Developmental Robotic 2005, Stanford, USA. pp. 6</t>
+  </si>
+  <si>
+    <t>Берем рекурентную сеть (LSM) с хаотическим поведением. Если там включить STDP, то нейроны синхронизируются, если anti-STDP то переходят в хаос. Если сихнронизацию включать при положительной награде, а десинхронизацию при отрицательно, то робот учится! Таинственно..</t>
   </si>
 </sst>
 </file>
@@ -6473,10 +6482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C93"/>
+  <dimension ref="A1:C94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="A93" sqref="A93"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="A94" sqref="A94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="44.1" customHeight="1"/>
@@ -7509,6 +7518,17 @@
       </c>
       <c r="C93" s="1" t="s">
         <v>2032</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A94" s="1" t="s">
+        <v>2033</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>2034</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>2035</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Synaptic Theory of Working Memory.pdf
</commit_message>
<xml_diff>
--- a/trunk/Список прочитанных статей.xlsx
+++ b/trunk/Список прочитанных статей.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2159" uniqueCount="2042">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2162" uniqueCount="2045">
   <si>
     <t>НАЗВАНИЕ</t>
   </si>
@@ -6143,6 +6143,15 @@
   </si>
   <si>
     <t>C. Boucheny, R. Carrillo, E. Ros and O. J.-M.D. Coenen; Computational Intelligence and Bioinspired Systems Lecture Notes in Computer Science, 2005, Volume 3512/2005,</t>
+  </si>
+  <si>
+    <t>Synaptic Theory of Working Memory</t>
+  </si>
+  <si>
+    <t>Mongillo G, Barak O, Tsodyks M.; Science. 2008;319:1543–6.</t>
+  </si>
+  <si>
+    <t>Теория рабочей памяти (кратковременной) на основе short-term placticity. Кальций копится в синапсах, если возбудить популяцию, а потом можно восстановить спайк популяции неспецифическим возбуждением. Разные данные хранятся в разных популяциях. Данные могут спонтанно реактивироваться от шума</t>
   </si>
 </sst>
 </file>
@@ -6498,10 +6507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C96"/>
+  <dimension ref="A1:C97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="B90" sqref="B90"/>
+      <selection activeCell="A97" sqref="A97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="44.1" customHeight="1"/>
@@ -7567,6 +7576,17 @@
       </c>
       <c r="C96" s="1" t="s">
         <v>2040</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A97" s="1" t="s">
+        <v>2042</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>2043</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>2044</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Spike-Timing Theory of Working Memory.pdf
</commit_message>
<xml_diff>
--- a/trunk/Список прочитанных статей.xlsx
+++ b/trunk/Список прочитанных статей.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2162" uniqueCount="2045">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2165" uniqueCount="2048">
   <si>
     <t>НАЗВАНИЕ</t>
   </si>
@@ -6152,6 +6152,15 @@
   </si>
   <si>
     <t>Теория рабочей памяти (кратковременной) на основе short-term placticity. Кальций копится в синапсах, если возбудить популяцию, а потом можно восстановить спайк популяции неспецифическим возбуждением. Разные данные хранятся в разных популяциях. Данные могут спонтанно реактивироваться от шума</t>
+  </si>
+  <si>
+    <t>Botond Szatmáry, Eugene M. Izhikevich</t>
+  </si>
+  <si>
+    <t>PLoS Comput Biol 6(8), 2010</t>
+  </si>
+  <si>
+    <t>Теория рабочей памяти на основе Polysynchronous neuronal group Ижикевича</t>
   </si>
 </sst>
 </file>
@@ -6507,10 +6516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C97"/>
+  <dimension ref="A1:C98"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="A97" sqref="A97"/>
+      <selection activeCell="B100" sqref="B100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="44.1" customHeight="1"/>
@@ -7587,6 +7596,17 @@
       </c>
       <c r="C97" s="1" t="s">
         <v>2044</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A98" t="s">
+        <v>2045</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>2046</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>2047</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- To beat or not to beat a decision taken at the network level
</commit_message>
<xml_diff>
--- a/trunk/Список прочитанных статей.xlsx
+++ b/trunk/Список прочитанных статей.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="10335" windowHeight="8385"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="10332" windowHeight="8388"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2165" uniqueCount="2048">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2168" uniqueCount="2051">
   <si>
     <t>НАЗВАНИЕ</t>
   </si>
@@ -6145,12 +6145,6 @@
     <t>Теория рабочей памяти (кратковременной) на основе short-term placticity. Кальций копится в синапсах, если возбудить популяцию, а потом можно восстановить спайк популяции неспецифическим возбуждением. Разные данные хранятся в разных популяциях. Данные могут спонтанно реактивироваться от шума</t>
   </si>
   <si>
-    <t>Botond Szatmáry, Eugene M. Izhikevich</t>
-  </si>
-  <si>
-    <t>PLoS Comput Biol 6(8), 2010</t>
-  </si>
-  <si>
     <t>Теория рабочей памяти на основе Polysynchronous neuronal group Ижикевича</t>
   </si>
   <si>
@@ -6161,13 +6155,30 @@
   </si>
   <si>
     <t>Краткий обзор симуляции миллиона нейронов Ижикевича</t>
+  </si>
+  <si>
+    <t>Botond Szatmáry, Eugene M. Izhikevich; PLoS Comput Biol 6(8), 2010</t>
+  </si>
+  <si>
+    <t>Spike-Timing Theory of Working Memory</t>
+  </si>
+  <si>
+    <t>To beat or not to beat: a decision taken at the network level</t>
+  </si>
+  <si>
+    <t>Manor et al.; J Physiol Paris (2000) vol. 94 (5-6) pp. 375-90</t>
+  </si>
+  <si>
+    <t>Gap juntions разиваюься в IO со времененм (в отличие от других мест, где они есть при рождении, а потом угасают). Это приводит к допороговым осциляциям напряжения с частотой ~6hz. Однако связь слабая, чтобы вызвать спайки только через нее. Гипотезы: electrical coupling is a
+mechanism of rhythmogenesis, Electrical coupling of heterogeneous neurons
+acts as a destabilizing factor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6182,6 +6193,14 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -6204,7 +6223,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -6222,6 +6241,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -6516,19 +6536,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C98"/>
+  <dimension ref="A1:C99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="C79" sqref="C79"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="B99" sqref="B99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="44.1" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="44.1" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="47.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="45.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="47.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="45.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="44.1" customHeight="1">
@@ -6649,7 +6669,7 @@
         <v>30</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>2045</v>
+        <v>2043</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="44.1" customHeight="1">
@@ -7045,7 +7065,7 @@
         <v>1890</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>2046</v>
+        <v>2044</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="44.1" customHeight="1">
@@ -7100,7 +7120,7 @@
         <v>1904</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>2047</v>
+        <v>2045</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="44.1" customHeight="1">
@@ -7599,14 +7619,25 @@
       </c>
     </row>
     <row r="98" spans="1:3" ht="44.1" customHeight="1">
-      <c r="A98" t="s">
+      <c r="A98" s="1" t="s">
+        <v>2047</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>2046</v>
+      </c>
+      <c r="C98" s="1" t="s">
         <v>2042</v>
       </c>
-      <c r="B98" s="1" t="s">
-        <v>2043</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>2044</v>
+    </row>
+    <row r="99" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A99" s="1" t="s">
+        <v>2048</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>2049</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>2050</v>
       </c>
     </row>
   </sheetData>
@@ -7623,12 +7654,12 @@
       <selection activeCell="A457" sqref="A457"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="44.1" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="44.1" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="47.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="64.42578125" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="47.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="64.44140625" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="44.1" customHeight="1">
@@ -14309,12 +14340,12 @@
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="96" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="96" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="33.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="69.28515625" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="33.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="27.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="69.33203125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="96" customHeight="1">

</xml_diff>

<commit_message>
- STDP/Spike-timing dependent synaptic plasticity a phenomenological framework.pdf
</commit_message>
<xml_diff>
--- a/trunk/Список прочитанных статей.xlsx
+++ b/trunk/Список прочитанных статей.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2168" uniqueCount="2051">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2171" uniqueCount="2054">
   <si>
     <t>НАЗВАНИЕ</t>
   </si>
@@ -6172,6 +6172,15 @@
     <t>Gap juntions разиваюься в IO со времененм (в отличие от других мест, где они есть при рождении, а потом угасают). Это приводит к допороговым осциляциям напряжения с частотой ~6hz. Однако связь слабая, чтобы вызвать спайки только через нее. Гипотезы: electrical coupling is a
 mechanism of rhythmogenesis, Electrical coupling of heterogeneous neurons
 acts as a destabilizing factor</t>
+  </si>
+  <si>
+    <t>Spike-timing dependent synaptic plasticity: a phenomenological framework</t>
+  </si>
+  <si>
+    <t>Kistler. W. M.; Biol Cybern (2002) vol. 87 (5-6) pp. 416-27</t>
+  </si>
+  <si>
+    <t>STDP служит для соревнований между входами: более надежные входы выигрывают, входы с большим разбросом во времени проигрывают. Также происходит стабилизация частоты через неассоциативные члены.</t>
   </si>
 </sst>
 </file>
@@ -6536,10 +6545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C99"/>
+  <dimension ref="A1:C100"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="B99" sqref="B99"/>
+      <selection activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="44.1" customHeight="1"/>
@@ -7638,6 +7647,17 @@
       </c>
       <c r="C99" s="1" t="s">
         <v>2050</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A100" s="1" t="s">
+        <v>2051</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>2052</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>2053</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cerebellum/Time windows and reverberating loops- a reverse-engineering approach to cerebellar function-Kistler 2003.pdf
</commit_message>
<xml_diff>
--- a/trunk/Список прочитанных статей.xlsx
+++ b/trunk/Список прочитанных статей.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2171" uniqueCount="2054">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2174" uniqueCount="2057">
   <si>
     <t>НАЗВАНИЕ</t>
   </si>
@@ -6181,6 +6181,15 @@
   </si>
   <si>
     <t>STDP служит для соревнований между входами: более надежные входы выигрывают, входы с большим разбросом во времени проигрывают. Также происходит стабилизация частоты через неассоциативные члены.</t>
+  </si>
+  <si>
+    <t>Time windows and reverberating loops- a reverse-engineering approach to cerebellar function</t>
+  </si>
+  <si>
+    <t>Kistler W. M., De Zeeuw CI.; Cerebellum. 2003;2(1):44-54.</t>
+  </si>
+  <si>
+    <t>Различные гипотезы про мозжечок. 1) Торможение от гольджи регулируют время а частоту granule, потому что их всего 4; 2) Rebound spike в dcn не возникает, если PC хаотичны. Если синхронизированы, то до спайка 100ms после снятия торможения. Время этого спайка очень устойчиво по отношению к количеству торможения. 3) Присутсвует паттерн: один вход получают пары клеток, а потом одни тормозят другие: mf -&gt; goldgi - gc; pf -&gt; pc - goldgi (pc тормозит glodgi); pf -&gt; bc - pc. Торможение чуть задерживается -&gt; Такие пары действуют как high-pass filter, пропускают только начало спайкового пакета.   4) IO действует как часы с частотой 10 Гц из за gap junctions. Этот сигнал уходит в mf и может быть использован всем мозжечком. А все эти feedbacks могут действовать как рабочая память на более длительный срок (на секунды).</t>
   </si>
 </sst>
 </file>
@@ -6545,10 +6554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C100"/>
+  <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="A100" sqref="A100"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="A102" sqref="A102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="44.1" customHeight="1"/>
@@ -7658,6 +7667,17 @@
       </c>
       <c r="C100" s="1" t="s">
         <v>2053</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A101" t="s">
+        <v>2054</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>2055</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>2056</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Dynamical working memory and timed responses the role of reverberating loops in the olivo-cerebellar system.pdf
</commit_message>
<xml_diff>
--- a/trunk/Список прочитанных статей.xlsx
+++ b/trunk/Список прочитанных статей.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2174" uniqueCount="2057">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2177" uniqueCount="2060">
   <si>
     <t>НАЗВАНИЕ</t>
   </si>
@@ -6190,6 +6190,15 @@
   </si>
   <si>
     <t>Различные гипотезы про мозжечок. 1) Торможение от гольджи регулируют время а частоту granule, потому что их всего 4; 2) Rebound spike в dcn не возникает, если PC хаотичны. Если синхронизированы, то до спайка 100ms после снятия торможения. Время этого спайка очень устойчиво по отношению к количеству торможения. 3) Присутсвует паттерн: один вход получают пары клеток, а потом одни тормозят другие: mf -&gt; goldgi - gc; pf -&gt; pc - goldgi (pc тормозит glodgi); pf -&gt; bc - pc. Торможение чуть задерживается -&gt; Такие пары действуют как high-pass filter, пропускают только начало спайкового пакета.   4) IO действует как часы с частотой 10 Гц из за gap junctions. Этот сигнал уходит в mf и может быть использован всем мозжечком. А все эти feedbacks могут действовать как рабочая память на более длительный срок (на секунды).</t>
+  </si>
+  <si>
+    <t>Dynamical working memory and timed responses: the role of reverberating loops in the olivo-cerebellar system</t>
+  </si>
+  <si>
+    <t>Kistler W. M., De Zeeuw CI. Neural computation (2002) vol. 14 (11) pp. 2597-626</t>
+  </si>
+  <si>
+    <t>Рекурентные сети в IO моделируются бинарными нейронами. Исследуются с помощью фазовых дискретных диаграмм. Интересная идея: сколько информации остается от первоначального паттерна после n ревербераций?</t>
   </si>
 </sst>
 </file>
@@ -6554,7 +6563,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C101"/>
+  <dimension ref="A1:C102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
       <selection activeCell="A102" sqref="A102"/>
@@ -7678,6 +7687,17 @@
       </c>
       <c r="C101" s="1" t="s">
         <v>2056</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A102" s="7" t="s">
+        <v>2057</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>2058</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>2059</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Regular patterns in cerebellar Purkinje cell simple spike trains.pdf
</commit_message>
<xml_diff>
--- a/trunk/Список прочитанных статей.xlsx
+++ b/trunk/Список прочитанных статей.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2177" uniqueCount="2060">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2180" uniqueCount="2063">
   <si>
     <t>НАЗВАНИЕ</t>
   </si>
@@ -6199,6 +6199,15 @@
   </si>
   <si>
     <t>Рекурентные сети в IO моделируются бинарными нейронами. Исследуются с помощью фазовых дискретных диаграмм. Интересная идея: сколько информации остается от первоначального паттерна после n ревербераций?</t>
+  </si>
+  <si>
+    <t>Regular patterns in cerebellar Purkinje cell simple spike trains</t>
+  </si>
+  <si>
+    <t>Shin et al. ,PLoS ONE (2007) vol. 2 (5) pp. e485</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Анализ выходных паттернов PC. Вывод: выход состоит из кусков регулярной частоты (разной) в 50ms, между которыми куски единичных спайков </t>
   </si>
 </sst>
 </file>
@@ -6563,10 +6572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C102"/>
+  <dimension ref="A1:C103"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="A102" sqref="A102"/>
+      <selection activeCell="A103" sqref="A103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="44.1" customHeight="1"/>
@@ -7698,6 +7707,17 @@
       </c>
       <c r="C102" s="1" t="s">
         <v>2059</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A103" s="1" t="s">
+        <v>2060</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>2061</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>2062</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Computational reconstruction of pacemaking and intrinsic electroresponsiveness in cerebellar golgi cells.pdf
</commit_message>
<xml_diff>
--- a/trunk/Список прочитанных статей.xlsx
+++ b/trunk/Список прочитанных статей.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2180" uniqueCount="2063">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2183" uniqueCount="2066">
   <si>
     <t>НАЗВАНИЕ</t>
   </si>
@@ -6208,6 +6208,15 @@
   </si>
   <si>
     <t xml:space="preserve">Анализ выходных паттернов PC. Вывод: выход состоит из кусков регулярной частоты (разной) в 50ms, между которыми куски единичных спайков </t>
+  </si>
+  <si>
+    <t>Computational reconstruction of pacemaking and intrinsic electroresponsiveness in cerebellar golgi cells</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S. Solinas, L. Forti, E. Cesana, J. Mapelli,E. De Schutter E. D'Angelo; Front Cell Neurosci. 2007; 1: 2. </t>
+  </si>
+  <si>
+    <t>Моделирование с помощьюканалов pacemaker activity of golgi cells</t>
   </si>
 </sst>
 </file>
@@ -6572,10 +6581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C103"/>
+  <dimension ref="A1:C104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="A103" sqref="A103"/>
+      <selection activeCell="A104" sqref="A104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="44.1" customHeight="1"/>
@@ -7718,6 +7727,17 @@
       </c>
       <c r="C103" s="1" t="s">
         <v>2062</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A104" s="1" t="s">
+        <v>2063</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>2064</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>2065</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Fast-Reset of Pacemaking and Theta-Frequency Resonance Patterns in Cerebellar Golgi Cells Simulations of their Impact In Vivo.pdf
</commit_message>
<xml_diff>
--- a/trunk/Список прочитанных статей.xlsx
+++ b/trunk/Список прочитанных статей.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2183" uniqueCount="2066">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2186" uniqueCount="2069">
   <si>
     <t>НАЗВАНИЕ</t>
   </si>
@@ -6216,7 +6216,16 @@
     <t xml:space="preserve">S. Solinas, L. Forti, E. Cesana, J. Mapelli,E. De Schutter E. D'Angelo; Front Cell Neurosci. 2007; 1: 2. </t>
   </si>
   <si>
-    <t>Моделирование с помощьюканалов pacemaker activity of golgi cells</t>
+    <t>Моделирование с помощьюканалов pacemaker activity of golgi cells (in vitro)</t>
+  </si>
+  <si>
+    <t>Fast-Reset of Pacemaking and Theta-Frequency Resonance Patterns in Cerebellar Golgi Cells: Simulations of their Impact In Vivo</t>
+  </si>
+  <si>
+    <t>S Solinas, L Forti, E Cesana, J Mapelli, E de Schutter, E D'Angelo; Front Cell Neurosci (2007) 1: 4</t>
+  </si>
+  <si>
+    <t>Pacemaker golgi in vitro becomes burst-pace makers in vivo under synaptic noise</t>
   </si>
 </sst>
 </file>
@@ -6581,10 +6590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C104"/>
+  <dimension ref="A1:C105"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="A104" sqref="A104"/>
+      <selection activeCell="A105" sqref="A105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="44.1" customHeight="1"/>
@@ -7738,6 +7747,17 @@
       </c>
       <c r="C104" s="1" t="s">
         <v>2065</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A105" s="1" t="s">
+        <v>2066</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>2067</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>2068</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- The Critical Role of Golgi Cells in Regulating Spatio-Temporal Integration and Plasticity at the Cerebellum Input Stage.pdf
</commit_message>
<xml_diff>
--- a/trunk/Список прочитанных статей.xlsx
+++ b/trunk/Список прочитанных статей.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2186" uniqueCount="2069">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2189" uniqueCount="2072">
   <si>
     <t>НАЗВАНИЕ</t>
   </si>
@@ -6226,6 +6226,15 @@
   </si>
   <si>
     <t>Pacemaker golgi in vitro becomes burst-pace makers in vivo under synaptic noise</t>
+  </si>
+  <si>
+    <t>The Critical Role of Golgi Cells in Regulating Spatio-Temporal Integration and Plasticity at the Cerebellum Input Stage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D'Angelo E.; Front Neurosci. 2008 July; 2(1): 35–46. </t>
+  </si>
+  <si>
+    <t>Отличный обзор Golgi cells. Все про connectivity, mediators, functional role. Гипотезы: делают области центр-периферия в пространстве mf. Обрезают непрерыную активность активность по времени с помощью этих зон. Не всегда осцилируют (в частности при  шумовом входе). При подаче длительного импульса - пачка pace bursts.</t>
   </si>
 </sst>
 </file>
@@ -6590,10 +6599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C105"/>
+  <dimension ref="A1:C106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
-      <selection activeCell="A105" sqref="A105"/>
+    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="A106" sqref="A106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="44.1" customHeight="1"/>
@@ -7758,6 +7767,17 @@
       </c>
       <c r="C105" s="1" t="s">
         <v>2068</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A106" s="1" t="s">
+        <v>2069</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>2070</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>2071</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Causes and Consequences of Oscillations in the Cerebellar Cortex.pdf
</commit_message>
<xml_diff>
--- a/trunk/Список прочитанных статей.xlsx
+++ b/trunk/Список прочитанных статей.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2195" uniqueCount="2077">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2198" uniqueCount="2080">
   <si>
     <t>НАЗВАНИЕ</t>
   </si>
@@ -6250,6 +6250,15 @@
   </si>
   <si>
     <t>Сопряженный градиент, онлайн градиент, эксперименты</t>
+  </si>
+  <si>
+    <t>Causes and Consequences of Oscillations in the Cerebellar Cortex</t>
+  </si>
+  <si>
+    <t>De Zeeuw CI, Hoebeek F.E., Schonewille M.; Neuron (2008) vol. 58 (5) pp. 655-8</t>
+  </si>
+  <si>
+    <t>Кратки обзор всевозможных осциляций в мозжечке</t>
   </si>
 </sst>
 </file>
@@ -6614,7 +6623,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C108"/>
+  <dimension ref="A1:C109"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
       <selection activeCell="A109" sqref="A109"/>
@@ -7815,6 +7824,17 @@
       </c>
       <c r="C108" s="1" t="s">
         <v>2076</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A109" s="1" t="s">
+        <v>2077</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>2078</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>2079</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Timing and plasticity in the cerebellum focus on the granular layer.pdf
</commit_message>
<xml_diff>
--- a/trunk/Список прочитанных статей.xlsx
+++ b/trunk/Список прочитанных статей.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2198" uniqueCount="2080">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2201" uniqueCount="2083">
   <si>
     <t>НАЗВАНИЕ</t>
   </si>
@@ -6259,6 +6259,15 @@
   </si>
   <si>
     <t>Кратки обзор всевозможных осциляций в мозжечке</t>
+  </si>
+  <si>
+    <t>Timing and plasticity in the cerebellum: focus on the granular layer.</t>
+  </si>
+  <si>
+    <t>D'Angelo E, De Zeeuw CI.; Trends Neurosci. 2009 Jan;32(1):30-40. Epub 2008 Oct 30.</t>
+  </si>
+  <si>
+    <t>Feedback to golgi: от PF, так как они влияют на выход gc. Feedforward to Golgi: from MF. BCM rule at mf-gc. Регулярность PC тоже важна, а не только интенсивность спайков на DCN для нормального  motor response. Приводит несколько фактов, что для поведения CF-PC пластичность не важна, а важна пластичность в granule layer!</t>
   </si>
 </sst>
 </file>
@@ -6623,10 +6632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C109"/>
+  <dimension ref="A1:C110"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="A109" sqref="A109"/>
+      <selection activeCell="A110" sqref="A110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="44.1" customHeight="1"/>
@@ -7835,6 +7844,17 @@
       </c>
       <c r="C109" s="1" t="s">
         <v>2079</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A110" s="1" t="s">
+        <v>2080</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>2081</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>2082</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Computational models of timing mechanisms in the cerebellar granular layer.pdf
</commit_message>
<xml_diff>
--- a/trunk/Список прочитанных статей.xlsx
+++ b/trunk/Список прочитанных статей.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2201" uniqueCount="2083">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2204" uniqueCount="2086">
   <si>
     <t>НАЗВАНИЕ</t>
   </si>
@@ -6268,6 +6268,15 @@
   </si>
   <si>
     <t>Feedback to golgi: от PF, так как они влияют на выход gc. Feedforward to Golgi: from MF. BCM rule at mf-gc. Регулярность PC тоже важна, а не только интенсивность спайков на DCN для нормального  motor response. Приводит несколько фактов, что для поведения CF-PC пластичность не важна, а важна пластичность в granule layer!</t>
+  </si>
+  <si>
+    <t>Yamazaki T., Tanaka S.; Cerebellum (2009) vol. 8 (4) pp. 423-32</t>
+  </si>
+  <si>
+    <t>Granule cells рекурентно тормозятся через GoC и случайные матрицы. Это позволяет на константный сигнал выдавать разные паттерны (LSM). Есть ссылка, что в PC есть механизм длительных медиаторов</t>
+  </si>
+  <si>
+    <t>Computational models of timing mechanisms in the cerebellar granular layer</t>
   </si>
 </sst>
 </file>
@@ -6632,10 +6641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C110"/>
+  <dimension ref="A1:C111"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="A110" sqref="A110"/>
+      <selection activeCell="A111" sqref="A111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="44.1" customHeight="1"/>
@@ -7855,6 +7864,17 @@
       </c>
       <c r="C110" s="1" t="s">
         <v>2082</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A111" s="1" t="s">
+        <v>2085</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>2083</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>2084</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Timing in the cerebellum oscillations and resonance in the granular layer.pdf
</commit_message>
<xml_diff>
--- a/trunk/Список прочитанных статей.xlsx
+++ b/trunk/Список прочитанных статей.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2204" uniqueCount="2086">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2207" uniqueCount="2089">
   <si>
     <t>НАЗВАНИЕ</t>
   </si>
@@ -6277,6 +6277,15 @@
   </si>
   <si>
     <t>Computational models of timing mechanisms in the cerebellar granular layer</t>
+  </si>
+  <si>
+    <t>Timing in the cerebellum: oscillations and resonance in the granular layer</t>
+  </si>
+  <si>
+    <t>D'angelo et al.; NSC (2009) pp. 1-11</t>
+  </si>
+  <si>
+    <t>Хороший обзор loops and oscillations в мозжечке в целом. Подробней про granule layer: GoC do time-windowing (5ms).</t>
   </si>
 </sst>
 </file>
@@ -6641,10 +6650,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C111"/>
+  <dimension ref="A1:C112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="A111" sqref="A111"/>
+    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
+      <selection activeCell="A112" sqref="A112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="44.1" customHeight="1"/>
@@ -7875,6 +7884,17 @@
       </c>
       <c r="C111" s="1" t="s">
         <v>2084</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A112" s="1" t="s">
+        <v>2086</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>2087</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>2088</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Elimination of climbing fiber instructive signals during motor learning.pdf
</commit_message>
<xml_diff>
--- a/trunk/Список прочитанных статей.xlsx
+++ b/trunk/Список прочитанных статей.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2207" uniqueCount="2089">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2210" uniqueCount="2092">
   <si>
     <t>НАЗВАНИЕ</t>
   </si>
@@ -6286,6 +6286,15 @@
   </si>
   <si>
     <t>Хороший обзор loops and oscillations в мозжечке в целом. Подробней про granule layer: GoC do time-windowing (5ms).</t>
+  </si>
+  <si>
+    <t>Elimination of climbing fiber instructive signals during motor learning</t>
+  </si>
+  <si>
+    <t>Ke M. C., Guo C.C., Raymond J.L. ; Nat Neurosci (2009) vol. 12 (9) pp. 1171-9</t>
+  </si>
+  <si>
+    <t>Ocullar Following Reflex можно обучаться без сигнала от CF, а только по активности PC. Что банально, если механизмы обучения ниже мозжечка.</t>
   </si>
 </sst>
 </file>
@@ -6650,10 +6659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C112"/>
+  <dimension ref="A1:C113"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="A112" sqref="A112"/>
+      <selection activeCell="C116" sqref="C116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="44.1" customHeight="1"/>
@@ -7895,6 +7904,17 @@
       </c>
       <c r="C112" s="1" t="s">
         <v>2088</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A113" s="1" t="s">
+        <v>2089</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>2090</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>2091</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- new articles portion
</commit_message>
<xml_diff>
--- a/trunk/Список прочитанных статей.xlsx
+++ b/trunk/Список прочитанных статей.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2210" uniqueCount="2092">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2228" uniqueCount="2109">
   <si>
     <t>НАЗВАНИЕ</t>
   </si>
@@ -6295,6 +6295,57 @@
   </si>
   <si>
     <t>Ocullar Following Reflex можно обучаться без сигнала от CF, а только по активности PC. Что банально, если механизмы обучения ниже мозжечка.</t>
+  </si>
+  <si>
+    <t>Sebastian A. Wills; PhD Disertation, Cambridge; 2004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сначала распознавание речи с помощью decaying rates: time-stretch invariant. Autoassociative temporal memory just like mine, but with veri artificial learning rules. Its capacity and linear atractor. </t>
+  </si>
+  <si>
+    <t>Paradigms for computing with spiking neurons</t>
+  </si>
+  <si>
+    <t>Различные варианты кодирования в spiking neurons: latency (показано, что они эквивалентно могут решать задачи из pereceptrons and backprop), enseble coding, и обзор других вариантов</t>
+  </si>
+  <si>
+    <t>Maass W.; from Models of Neural Networks IV: Early Vision and Attention by J. Leo van Hemmen, Jack D. Cowan, and Eytan Domany; 2001</t>
+  </si>
+  <si>
+    <t>Policy-Gradient Algorithms for Partially Observable Markov Decision Processes</t>
+  </si>
+  <si>
+    <t>Aberdeen D.A. PhD disertation; Australian national university (2003)</t>
+  </si>
+  <si>
+    <t>Диссертация по управлению с памятью POMDP. Очень отличная. Про градиент по памяти, сравнение разных алгоритмов обучения POMDP, примеры, теоремы и тд</t>
+  </si>
+  <si>
+    <t>A Biologically Plausible and Locally Optimal Learning Algorithm for Spiking Neurons</t>
+  </si>
+  <si>
+    <t>Bartlett P., Baxter J. http://arp.anu.edu.au/ftp/papers/jon/brains.pdf.gz, 2000</t>
+  </si>
+  <si>
+    <t>Краткая статья OLPOMDP для стохастических персептронов</t>
+  </si>
+  <si>
+    <t>Infinite-Horizon Policy-Gradient Estimation</t>
+  </si>
+  <si>
+    <t>Их основные результаты только по простому градиенту, с расширенной частью про топологические теоремы</t>
+  </si>
+  <si>
+    <t>Baxter J. , Bartlett P.; Journal of Artificial Intelligence Research 2001</t>
+  </si>
+  <si>
+    <t>Efficient Gradient Estimation for Motor Control Learning</t>
+  </si>
+  <si>
+    <t>Lawrence G., Cowan N., Russell S.; Proceedings of the Proceedings of the Nineteenth Conference Annual Conference on Uncertainty in Artificial Intelligence (UAI-03); 2003</t>
+  </si>
+  <si>
+    <t>Стохастический градиент по политикам по идеям REINFORCE + спецальные методики для уменьшения дисперсии. На задаче метания ядра и дротика.</t>
   </si>
 </sst>
 </file>
@@ -6659,10 +6710,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C113"/>
+  <dimension ref="A1:C119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" workbookViewId="0">
-      <selection activeCell="C116" sqref="C116"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="B120" sqref="B120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="44.1" customHeight="1"/>
@@ -7915,6 +7966,72 @@
       </c>
       <c r="C113" s="1" t="s">
         <v>2091</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A114" s="1" t="s">
+        <v>1862</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>2092</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>2093</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A115" s="1" t="s">
+        <v>2094</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>2096</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>2095</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A116" s="1" t="s">
+        <v>2097</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>2098</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>2099</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A117" s="1" t="s">
+        <v>2100</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>2101</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>2102</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A118" s="1" t="s">
+        <v>2103</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>2105</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>2104</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A119" s="1" t="s">
+        <v>2106</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>2107</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>2108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- a focused backprop
</commit_message>
<xml_diff>
--- a/trunk/Список прочитанных статей.xlsx
+++ b/trunk/Список прочитанных статей.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2228" uniqueCount="2109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2231" uniqueCount="2112">
   <si>
     <t>НАЗВАНИЕ</t>
   </si>
@@ -6346,6 +6346,15 @@
   </si>
   <si>
     <t>Стохастический градиент по политикам по идеям REINFORCE + спецальные методики для уменьшения дисперсии. На задаче метания ядра и дротика.</t>
+  </si>
+  <si>
+    <t>Mozer, M. C.; Hillsdale, NJ: Lawrence Erlbaum Associates. pp. 137–169., 1995</t>
+  </si>
+  <si>
+    <t>a focused backpropagation algorithm for temporal pattern recognition</t>
+  </si>
+  <si>
+    <t>Обратное распространение в рекурсивных сетях - сеть разлагается по времени в кучу слоев, потом простой backprop. Но ошибка сильно размывается к последним слоям. Для этого он вводит подобие eligibility traces для фокусировки ошибки</t>
   </si>
 </sst>
 </file>
@@ -6710,10 +6719,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C119"/>
+  <dimension ref="A1:C120"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="B120" sqref="B120"/>
+      <selection activeCell="A121" sqref="A121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="44.1" customHeight="1"/>
@@ -8032,6 +8041,17 @@
       </c>
       <c r="C119" s="1" t="s">
         <v>2108</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" ht="44.1" customHeight="1">
+      <c r="A120" s="1" t="s">
+        <v>2110</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>2109</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>2111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>